<commit_message>
Drug rule messages update.
</commit_message>
<xml_diff>
--- a/CDS_Medication-Condition_Cards.xlsx
+++ b/CDS_Medication-Condition_Cards.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Contraindication: {{ActualMedication}} with patient condition {{ActualCondition}}.</t>
   </si>
   <si>
-    <t xml:space="preserve">The use of {{Medication}} is contraindicated when the patient has {{Condition}}.</t>
+    <t xml:space="preserve">The use of {{RuleMedication}} is contraindicated when the patient has {{RuleCondition}}.</t>
   </si>
   <si>
     <t xml:space="preserve">Wikipedia</t>
@@ -260,7 +260,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,8 +269,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="17.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="51.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.24"/>
@@ -313,7 +314,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="92" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -346,7 +347,7 @@
       </c>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -378,7 +379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -410,7 +411,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -442,7 +443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>